<commit_message>
Added new sheet named Education
</commit_message>
<xml_diff>
--- a/MarsQA-1/SpecflowTests/Data/Data.xlsx
+++ b/MarsQA-1/SpecflowTests/Data/Data.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7121D064-FA83-4CD1-9057-21A69B20E80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6EA9DE-53FB-45C4-9726-A02B94A9AF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Language" sheetId="1" r:id="rId1"/>
     <sheet name="Skills" sheetId="2" r:id="rId2"/>
+    <sheet name="Education" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>Language</t>
   </si>
@@ -73,6 +74,114 @@
   </si>
   <si>
     <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Graduation Year</t>
+  </si>
+  <si>
+    <t>Nagpur University</t>
+  </si>
+  <si>
+    <t>NIU</t>
+  </si>
+  <si>
+    <t>Harward</t>
+  </si>
+  <si>
+    <t>Victoria University</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>B.Tech</t>
+  </si>
+  <si>
+    <t>M.Tech</t>
+  </si>
+  <si>
+    <t>M.B.A</t>
+  </si>
+  <si>
+    <t>PHD</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT </t>
+  </si>
+  <si>
+    <t>B.A</t>
+  </si>
+  <si>
+    <t>BFA</t>
+  </si>
+  <si>
+    <t>M.A</t>
+  </si>
+  <si>
+    <t>B.Sc</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>PTU</t>
+  </si>
+  <si>
+    <t>STU</t>
+  </si>
+  <si>
+    <t>KYU</t>
+  </si>
+  <si>
+    <t>RRU</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>Physcology</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Japan</t>
   </si>
 </sst>
 </file>
@@ -466,7 +575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -559,7 +668,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,4 +769,180 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F11439-867B-4031-80D5-818971F26D6C}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <v>2021</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>